<commit_message>
JSON schema exporter updated.
</commit_message>
<xml_diff>
--- a/schema_definitions/study_schema_v1.0.xlsx
+++ b/schema_definitions/study_schema_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1A6F07-C5BA-9540-9B6F-A300659F579C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E8D737-A7BC-124E-82D2-CBECE5B8794B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35440" yWindow="-1520" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="28800" yWindow="-4160" windowWidth="51200" windowHeight="28340" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>NAME</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ACCEPTED</t>
   </si>
   <si>
-    <t>CURRENTLY_SUPPORTED</t>
-  </si>
-  <si>
     <t>study_tag</t>
   </si>
   <si>
@@ -117,12 +114,6 @@
     <t>Genome-wide genotyping array|Targeted genotyping array|Exome genotyping array|Whole genome sequencing</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Manufacturer of the genotyping array used for the discovery stage</t>
   </si>
   <si>
@@ -186,9 +177,6 @@
     <t>Yes|No</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>The number of variants analysed in the discovery stage (after QC)</t>
   </si>
   <si>
@@ -199,9 +187,6 @@
   </si>
   <si>
     <t>Any background trait(s) shared by all individuals in the GWAS (e.g. in both cases and controls)</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>EFOs that best match entered “background trait”</t>
@@ -628,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +630,7 @@
     <col min="11" max="11" width="96" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -679,377 +664,338 @@
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="3" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="J6" t="s">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
         <v>38</v>
       </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>67</v>
       </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="J16" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" t="s">
-        <v>62</v>
-      </c>
-      <c r="L16" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>